<commit_message>
Adjust mean variance catch per trip
</commit_message>
<xml_diff>
--- a/sf_fitted_sizes_y2plus.xlsx
+++ b/sf_fitted_sizes_y2plus.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D99"/>
+  <dimension ref="A1:D101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -381,7 +381,7 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>6.972750189097953e-006</v>
+        <v>5.76009798229831e-006</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -399,7 +399,7 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>0.0002094856687246385</v>
+        <v>0.0002049382229491399</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -417,7 +417,7 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>0.002126688807674876</v>
+        <v>0.002090612404522586</v>
       </c>
       <c r="B4">
         <v>4</v>
@@ -435,7 +435,7 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>0.009901608431570794</v>
+        <v>0.00991646342110409</v>
       </c>
       <c r="B5">
         <v>5</v>
@@ -453,7 +453,7 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>0.0289423702196871</v>
+        <v>0.02874319209472026</v>
       </c>
       <c r="B6">
         <v>6</v>
@@ -471,7 +471,7 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>0.0596161046276324</v>
+        <v>0.05919016053999403</v>
       </c>
       <c r="B7">
         <v>7</v>
@@ -489,7 +489,7 @@
     </row>
     <row r="8">
       <c r="A8">
-        <v>0.09440558062545569</v>
+        <v>0.0943801149291129</v>
       </c>
       <c r="B8">
         <v>8</v>
@@ -507,7 +507,7 @@
     </row>
     <row r="9">
       <c r="A9">
-        <v>0.1230663123701136</v>
+        <v>0.1228489444620447</v>
       </c>
       <c r="B9">
         <v>9</v>
@@ -525,7 +525,7 @@
     </row>
     <row r="10">
       <c r="A10">
-        <v>0.1365867781498262</v>
+        <v>0.1367159256098504</v>
       </c>
       <c r="B10">
         <v>10</v>
@@ -543,7 +543,7 @@
     </row>
     <row r="11">
       <c r="A11">
-        <v>0.1338631612933542</v>
+        <v>0.1337776693127749</v>
       </c>
       <c r="B11">
         <v>11</v>
@@ -561,7 +561,7 @@
     </row>
     <row r="12">
       <c r="A12">
-        <v>0.1173013637789881</v>
+        <v>0.1176133185591873</v>
       </c>
       <c r="B12">
         <v>12</v>
@@ -579,7 +579,7 @@
     </row>
     <row r="13">
       <c r="A13">
-        <v>0.0943910287989741</v>
+        <v>0.09474360742810109</v>
       </c>
       <c r="B13">
         <v>13</v>
@@ -597,7 +597,7 @@
     </row>
     <row r="14">
       <c r="A14">
-        <v>0.07020195206688989</v>
+        <v>0.07069216672148865</v>
       </c>
       <c r="B14">
         <v>14</v>
@@ -615,7 +615,7 @@
     </row>
     <row r="15">
       <c r="A15">
-        <v>0.04926278324902874</v>
+        <v>0.049085736026836</v>
       </c>
       <c r="B15">
         <v>15</v>
@@ -633,7 +633,7 @@
     </row>
     <row r="16">
       <c r="A16">
-        <v>0.03251181199040186</v>
+        <v>0.03226170247274943</v>
       </c>
       <c r="B16">
         <v>16</v>
@@ -651,7 +651,7 @@
     </row>
     <row r="17">
       <c r="A17">
-        <v>0.02021642810260857</v>
+        <v>0.02039711328142171</v>
       </c>
       <c r="B17">
         <v>17</v>
@@ -669,7 +669,7 @@
     </row>
     <row r="18">
       <c r="A18">
-        <v>0.01214895613382223</v>
+        <v>0.0122587011585376</v>
       </c>
       <c r="B18">
         <v>18</v>
@@ -687,7 +687,7 @@
     </row>
     <row r="19">
       <c r="A19">
-        <v>0.007098866018605116</v>
+        <v>0.006953347753789159</v>
       </c>
       <c r="B19">
         <v>19</v>
@@ -705,7 +705,7 @@
     </row>
     <row r="20">
       <c r="A20">
-        <v>0.003913531834394152</v>
+        <v>0.003888369301103059</v>
       </c>
       <c r="B20">
         <v>20</v>
@@ -723,7 +723,7 @@
     </row>
     <row r="21">
       <c r="A21">
-        <v>0.002076363741092691</v>
+        <v>0.002060296099352595</v>
       </c>
       <c r="B21">
         <v>21</v>
@@ -741,7 +741,7 @@
     </row>
     <row r="22">
       <c r="A22">
-        <v>0.001070165572500686</v>
+        <v>0.001103816671239376</v>
       </c>
       <c r="B22">
         <v>22</v>
@@ -759,7 +759,7 @@
     </row>
     <row r="23">
       <c r="A23">
-        <v>0.0005644896022652344</v>
+        <v>0.0005350827862503429</v>
       </c>
       <c r="B23">
         <v>23</v>
@@ -777,7 +777,7 @@
     </row>
     <row r="24">
       <c r="A24">
-        <v>0.0002667834854959217</v>
+        <v>0.0002883080621666154</v>
       </c>
       <c r="B24">
         <v>24</v>
@@ -795,7 +795,7 @@
     </row>
     <row r="25">
       <c r="A25">
-        <v>0.0001318759274894613</v>
+        <v>0.0001264189925588629</v>
       </c>
       <c r="B25">
         <v>25</v>
@@ -813,7 +813,7 @@
     </row>
     <row r="26">
       <c r="A26">
-        <v>6.032944728828229e-005</v>
+        <v>6.245158865018167e-005</v>
       </c>
       <c r="B26">
         <v>26</v>
@@ -831,7 +831,7 @@
     </row>
     <row r="27">
       <c r="A27">
-        <v>3.365109873869012e-005</v>
+        <v>3.061946822169101e-005</v>
       </c>
       <c r="B27">
         <v>27</v>
@@ -849,7 +849,7 @@
     </row>
     <row r="28">
       <c r="A28">
-        <v>1.333917427479609e-005</v>
+        <v>1.394550037819591e-005</v>
       </c>
       <c r="B28">
         <v>28</v>
@@ -867,7 +867,7 @@
     </row>
     <row r="29">
       <c r="A29">
-        <v>5.456934930598399e-006</v>
+        <v>6.972750189097953e-006</v>
       </c>
       <c r="B29">
         <v>29</v>
@@ -885,7 +885,7 @@
     </row>
     <row r="30">
       <c r="A30">
-        <v>3.637956620398932e-006</v>
+        <v>2.728467465299199e-006</v>
       </c>
       <c r="B30">
         <v>30</v>
@@ -903,7 +903,7 @@
     </row>
     <row r="31">
       <c r="A31">
-        <v>1.515815258499555e-006</v>
+        <v>9.09489155099733e-007</v>
       </c>
       <c r="B31">
         <v>31</v>
@@ -921,10 +921,10 @@
     </row>
     <row r="32">
       <c r="A32">
-        <v>3.03163051699911e-007</v>
+        <v>6.063261033998221e-007</v>
       </c>
       <c r="B32">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -939,14 +939,14 @@
     </row>
     <row r="33">
       <c r="A33">
-        <v>3.03163051699911e-007</v>
+        <v>8.953487705786961e-008</v>
       </c>
       <c r="B33">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>SO</t>
+          <t>NJ</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -957,7 +957,7 @@
     </row>
     <row r="34">
       <c r="A34">
-        <v>3.760464836430524e-006</v>
+        <v>4.208139221719872e-006</v>
       </c>
       <c r="B34">
         <v>4</v>
@@ -975,7 +975,7 @@
     </row>
     <row r="35">
       <c r="A35">
-        <v>9.598138820603622e-005</v>
+        <v>9.633952771426771e-005</v>
       </c>
       <c r="B35">
         <v>5</v>
@@ -993,7 +993,7 @@
     </row>
     <row r="36">
       <c r="A36">
-        <v>0.0009268650473030662</v>
+        <v>0.0008909615616028606</v>
       </c>
       <c r="B36">
         <v>6</v>
@@ -1011,7 +1011,7 @@
     </row>
     <row r="37">
       <c r="A37">
-        <v>0.004812410106983434</v>
+        <v>0.004885739171293829</v>
       </c>
       <c r="B37">
         <v>7</v>
@@ -1029,7 +1029,7 @@
     </row>
     <row r="38">
       <c r="A38">
-        <v>0.0165834708589045</v>
+        <v>0.01656780225541937</v>
       </c>
       <c r="B38">
         <v>8</v>
@@ -1047,7 +1047,7 @@
     </row>
     <row r="39">
       <c r="A39">
-        <v>0.04047450977864113</v>
+        <v>0.04061257255906437</v>
       </c>
       <c r="B39">
         <v>9</v>
@@ -1065,7 +1065,7 @@
     </row>
     <row r="40">
       <c r="A40">
-        <v>0.07511206185212563</v>
+        <v>0.07491687582013948</v>
       </c>
       <c r="B40">
         <v>10</v>
@@ -1083,7 +1083,7 @@
     </row>
     <row r="41">
       <c r="A41">
-        <v>0.1114531940313902</v>
+        <v>0.1114943800748368</v>
       </c>
       <c r="B41">
         <v>11</v>
@@ -1101,7 +1101,7 @@
     </row>
     <row r="42">
       <c r="A42">
-        <v>0.1376034665039281</v>
+        <v>0.1375617432512191</v>
       </c>
       <c r="B42">
         <v>12</v>
@@ -1119,7 +1119,7 @@
     </row>
     <row r="43">
       <c r="A43">
-        <v>0.1458302891475134</v>
+        <v>0.1458144414742741</v>
       </c>
       <c r="B43">
         <v>13</v>
@@ -1137,7 +1137,7 @@
     </row>
     <row r="44">
       <c r="A44">
-        <v>0.1350775085523715</v>
+        <v>0.1348603864755061</v>
       </c>
       <c r="B44">
         <v>14</v>
@@ -1155,7 +1155,7 @@
     </row>
     <row r="45">
       <c r="A45">
-        <v>0.1114052033372872</v>
+        <v>0.1114221254290511</v>
       </c>
       <c r="B45">
         <v>15</v>
@@ -1173,7 +1173,7 @@
     </row>
     <row r="46">
       <c r="A46">
-        <v>0.08310099032736816</v>
+        <v>0.08329966821955957</v>
       </c>
       <c r="B46">
         <v>16</v>
@@ -1191,7 +1191,7 @@
     </row>
     <row r="47">
       <c r="A47">
-        <v>0.05686207832654301</v>
+        <v>0.05695098645946147</v>
       </c>
       <c r="B47">
         <v>17</v>
@@ -1209,7 +1209,7 @@
     </row>
     <row r="48">
       <c r="A48">
-        <v>0.03593043569820013</v>
+        <v>0.0358907717476635</v>
       </c>
       <c r="B48">
         <v>18</v>
@@ -1227,7 +1227,7 @@
     </row>
     <row r="49">
       <c r="A49">
-        <v>0.0211912937718107</v>
+        <v>0.02122173563001037</v>
       </c>
       <c r="B49">
         <v>19</v>
@@ -1245,7 +1245,7 @@
     </row>
     <row r="50">
       <c r="A50">
-        <v>0.01178189447204506</v>
+        <v>0.0117123258725711</v>
       </c>
       <c r="B50">
         <v>20</v>
@@ -1263,7 +1263,7 @@
     </row>
     <row r="51">
       <c r="A51">
-        <v>0.006135108845759342</v>
+        <v>0.006141734426661624</v>
       </c>
       <c r="B51">
         <v>21</v>
@@ -1281,7 +1281,7 @@
     </row>
     <row r="52">
       <c r="A52">
-        <v>0.003032188146441813</v>
+        <v>0.003052602098411007</v>
       </c>
       <c r="B52">
         <v>22</v>
@@ -1299,7 +1299,7 @@
     </row>
     <row r="53">
       <c r="A53">
-        <v>0.001463537100387937</v>
+        <v>0.001457448728748002</v>
       </c>
       <c r="B53">
         <v>23</v>
@@ -1317,7 +1317,7 @@
     </row>
     <row r="54">
       <c r="A54">
-        <v>0.000644830184570777</v>
+        <v>0.0006530673932601009</v>
       </c>
       <c r="B54">
         <v>24</v>
@@ -1335,7 +1335,7 @@
     </row>
     <row r="55">
       <c r="A55">
-        <v>0.0002806918395764213</v>
+        <v>0.0002867802112163564</v>
       </c>
       <c r="B55">
         <v>25</v>
@@ -1353,7 +1353,7 @@
     </row>
     <row r="56">
       <c r="A56">
-        <v>0.0001172011540687513</v>
+        <v>0.0001258860371433647</v>
       </c>
       <c r="B56">
         <v>26</v>
@@ -1371,7 +1371,7 @@
     </row>
     <row r="57">
       <c r="A57">
-        <v>5.040813578358059e-005</v>
+        <v>5.094534504592781e-005</v>
       </c>
       <c r="B57">
         <v>27</v>
@@ -1389,7 +1389,7 @@
     </row>
     <row r="58">
       <c r="A58">
-        <v>1.933953344449984e-005</v>
+        <v>1.835464979686327e-005</v>
       </c>
       <c r="B58">
         <v>28</v>
@@ -1407,7 +1407,7 @@
     </row>
     <row r="59">
       <c r="A59">
-        <v>7.520929672861047e-006</v>
+        <v>6.356976271108742e-006</v>
       </c>
       <c r="B59">
         <v>29</v>
@@ -1425,7 +1425,7 @@
     </row>
     <row r="60">
       <c r="A60">
-        <v>2.238371926446741e-006</v>
+        <v>2.775581188793958e-006</v>
       </c>
       <c r="B60">
         <v>30</v>
@@ -1443,7 +1443,7 @@
     </row>
     <row r="61">
       <c r="A61">
-        <v>1.074418524694435e-006</v>
+        <v>6.267441394050873e-007</v>
       </c>
       <c r="B61">
         <v>31</v>
@@ -1461,7 +1461,7 @@
     </row>
     <row r="62">
       <c r="A62">
-        <v>2.686046311736089e-007</v>
+        <v>1.790697541157392e-007</v>
       </c>
       <c r="B62">
         <v>32</v>
@@ -1479,10 +1479,10 @@
     </row>
     <row r="63">
       <c r="A63">
-        <v>1.790697541157392e-007</v>
+        <v>8.953487705786961e-008</v>
       </c>
       <c r="B63">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
@@ -1497,7 +1497,7 @@
     </row>
     <row r="64">
       <c r="A64">
-        <v>9.886249798444082e-008</v>
+        <v>2.965874939533225e-007</v>
       </c>
       <c r="B64">
         <v>3</v>
@@ -1533,7 +1533,7 @@
     </row>
     <row r="66">
       <c r="A66">
-        <v>0.0001421642721016259</v>
+        <v>0.0001474039844948013</v>
       </c>
       <c r="B66">
         <v>5</v>
@@ -1551,7 +1551,7 @@
     </row>
     <row r="67">
       <c r="A67">
-        <v>0.001032223341455547</v>
+        <v>0.001041318691270115</v>
       </c>
       <c r="B67">
         <v>6</v>
@@ -1569,7 +1569,7 @@
     </row>
     <row r="68">
       <c r="A68">
-        <v>0.004506053795632828</v>
+        <v>0.004535020507542269</v>
       </c>
       <c r="B68">
         <v>7</v>
@@ -1587,7 +1587,7 @@
     </row>
     <row r="69">
       <c r="A69">
-        <v>0.01360931261004014</v>
+        <v>0.01364302472185283</v>
       </c>
       <c r="B69">
         <v>8</v>
@@ -1605,7 +1605,7 @@
     </row>
     <row r="70">
       <c r="A70">
-        <v>0.03101099064276343</v>
+        <v>0.03098756023074112</v>
       </c>
       <c r="B70">
         <v>9</v>
@@ -1623,7 +1623,7 @@
     </row>
     <row r="71">
       <c r="A71">
-        <v>0.05610021651875684</v>
+        <v>0.05605711246963562</v>
       </c>
       <c r="B71">
         <v>10</v>
@@ -1641,7 +1641,7 @@
     </row>
     <row r="72">
       <c r="A72">
-        <v>0.08438813851703683</v>
+        <v>0.08436006156760925</v>
       </c>
       <c r="B72">
         <v>11</v>
@@ -1659,7 +1659,7 @@
     </row>
     <row r="73">
       <c r="A73">
-        <v>0.108843556918452</v>
+        <v>0.1088147879315385</v>
       </c>
       <c r="B73">
         <v>12</v>
@@ -1677,7 +1677,7 @@
     </row>
     <row r="74">
       <c r="A74">
-        <v>0.1231789157136899</v>
+        <v>0.1233106994235031</v>
       </c>
       <c r="B74">
         <v>13</v>
@@ -1695,7 +1695,7 @@
     </row>
     <row r="75">
       <c r="A75">
-        <v>0.1251951174975846</v>
+        <v>0.1251313511863846</v>
       </c>
       <c r="B75">
         <v>14</v>
@@ -1713,7 +1713,7 @@
     </row>
     <row r="76">
       <c r="A76">
-        <v>0.1152105983761439</v>
+        <v>0.1151857838891498</v>
       </c>
       <c r="B76">
         <v>15</v>
@@ -1731,7 +1731,7 @@
     </row>
     <row r="77">
       <c r="A77">
-        <v>0.09787337869210649</v>
+        <v>0.09758984104788712</v>
       </c>
       <c r="B77">
         <v>16</v>
@@ -1749,7 +1749,7 @@
     </row>
     <row r="78">
       <c r="A78">
-        <v>0.07689653614477186</v>
+        <v>0.07706084561642201</v>
       </c>
       <c r="B78">
         <v>17</v>
@@ -1767,7 +1767,7 @@
     </row>
     <row r="79">
       <c r="A79">
-        <v>0.05678128026737165</v>
+        <v>0.05701469462511291</v>
       </c>
       <c r="B79">
         <v>18</v>
@@ -1785,7 +1785,7 @@
     </row>
     <row r="80">
       <c r="A80">
-        <v>0.03965355021656324</v>
+        <v>0.0396748056536299</v>
       </c>
       <c r="B80">
         <v>19</v>
@@ -1803,7 +1803,7 @@
     </row>
     <row r="81">
       <c r="A81">
-        <v>0.02623800810257261</v>
+        <v>0.02619332225348364</v>
       </c>
       <c r="B81">
         <v>20</v>
@@ -1821,7 +1821,7 @@
     </row>
     <row r="82">
       <c r="A82">
-        <v>0.01660336336149893</v>
+        <v>0.0164980748011455</v>
       </c>
       <c r="B82">
         <v>21</v>
@@ -1839,7 +1839,7 @@
     </row>
     <row r="83">
       <c r="A83">
-        <v>0.01001734147077145</v>
+        <v>0.009992724708773325</v>
       </c>
       <c r="B83">
         <v>22</v>
@@ -1857,7 +1857,7 @@
     </row>
     <row r="84">
       <c r="A84">
-        <v>0.005792057169414435</v>
+        <v>0.005828636293668678</v>
       </c>
       <c r="B84">
         <v>23</v>
@@ -1875,7 +1875,7 @@
     </row>
     <row r="85">
       <c r="A85">
-        <v>0.003257618171085309</v>
+        <v>0.003260485183526858</v>
       </c>
       <c r="B85">
         <v>24</v>
@@ -1893,7 +1893,7 @@
     </row>
     <row r="86">
       <c r="A86">
-        <v>0.001780019276209857</v>
+        <v>0.001792673675951866</v>
       </c>
       <c r="B86">
         <v>25</v>
@@ -1911,7 +1911,7 @@
     </row>
     <row r="87">
       <c r="A87">
-        <v>0.0009368210309005612</v>
+        <v>0.0009433459557675343</v>
       </c>
       <c r="B87">
         <v>26</v>
@@ -1929,7 +1929,7 @@
     </row>
     <row r="88">
       <c r="A88">
-        <v>0.0004836353401398845</v>
+        <v>0.000476121790293067</v>
       </c>
       <c r="B88">
         <v>27</v>
@@ -1947,7 +1947,7 @@
     </row>
     <row r="89">
       <c r="A89">
-        <v>0.0002410267700860667</v>
+        <v>0.0002325245952594048</v>
       </c>
       <c r="B89">
         <v>28</v>
@@ -1965,7 +1965,7 @@
     </row>
     <row r="90">
       <c r="A90">
-        <v>0.0001133952851881536</v>
+        <v>0.0001138895976780758</v>
       </c>
       <c r="B90">
         <v>29</v>
@@ -1983,7 +1983,7 @@
     </row>
     <row r="91">
       <c r="A91">
-        <v>5.476982388338022e-005</v>
+        <v>5.743911132896012e-005</v>
       </c>
       <c r="B91">
         <v>30</v>
@@ -2001,7 +2001,7 @@
     </row>
     <row r="92">
       <c r="A92">
-        <v>2.708832444773679e-005</v>
+        <v>2.392472451223468e-005</v>
       </c>
       <c r="B92">
         <v>31</v>
@@ -2019,7 +2019,7 @@
     </row>
     <row r="93">
       <c r="A93">
-        <v>1.384074971782172e-005</v>
+        <v>1.057828728433517e-005</v>
       </c>
       <c r="B93">
         <v>32</v>
@@ -2037,7 +2037,7 @@
     </row>
     <row r="94">
       <c r="A94">
-        <v>5.140849895190923e-006</v>
+        <v>5.338574891159804e-006</v>
       </c>
       <c r="B94">
         <v>33</v>
@@ -2055,7 +2055,7 @@
     </row>
     <row r="95">
       <c r="A95">
-        <v>1.878387461704376e-006</v>
+        <v>3.262462433486547e-006</v>
       </c>
       <c r="B95">
         <v>34</v>
@@ -2073,7 +2073,7 @@
     </row>
     <row r="96">
       <c r="A96">
-        <v>8.897624818599675e-007</v>
+        <v>1.680662465735494e-006</v>
       </c>
       <c r="B96">
         <v>35</v>
@@ -2091,7 +2091,7 @@
     </row>
     <row r="97">
       <c r="A97">
-        <v>3.954499919377633e-007</v>
+        <v>4.943124899222041e-007</v>
       </c>
       <c r="B97">
         <v>36</v>
@@ -2127,7 +2127,7 @@
     </row>
     <row r="99">
       <c r="A99">
-        <v>9.886249798444082e-008</v>
+        <v>1.977249959688816e-007</v>
       </c>
       <c r="B99">
         <v>38</v>
@@ -2138,6 +2138,42 @@
         </is>
       </c>
       <c r="D99" t="inlineStr">
+        <is>
+          <t>y2</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100">
+        <v>9.886249798444082e-008</v>
+      </c>
+      <c r="B100">
+        <v>39</v>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>y2</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101">
+        <v>9.886249798444082e-008</v>
+      </c>
+      <c r="B101">
+        <v>40</v>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
         <is>
           <t>y2</t>
         </is>

</xml_diff>

<commit_message>
create new catch @ length without smoothing
</commit_message>
<xml_diff>
--- a/sf_fitted_sizes_y2plus.xlsx
+++ b/sf_fitted_sizes_y2plus.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D101"/>
+  <dimension ref="A1:D66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -381,10 +381,10 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>5.76009798229831e-006</v>
+        <v>0.03220971889174588</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -399,10 +399,10 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>0.0002049382229491399</v>
+        <v>0.05415274286796547</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -417,10 +417,10 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>0.002090612404522586</v>
+        <v>0.07296511907857356</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -435,10 +435,10 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>0.00991646342110409</v>
+        <v>0.07448871169149678</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -453,10 +453,10 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>0.02874319209472026</v>
+        <v>0.1740266181299897</v>
       </c>
       <c r="B6">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -471,10 +471,10 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>0.05919016053999403</v>
+        <v>0.229409229672859</v>
       </c>
       <c r="B7">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -489,10 +489,10 @@
     </row>
     <row r="8">
       <c r="A8">
-        <v>0.0943801149291129</v>
+        <v>0.0948656092604898</v>
       </c>
       <c r="B8">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -507,10 +507,10 @@
     </row>
     <row r="9">
       <c r="A9">
-        <v>0.1228489444620447</v>
+        <v>0.06609952265847449</v>
       </c>
       <c r="B9">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -525,10 +525,10 @@
     </row>
     <row r="10">
       <c r="A10">
-        <v>0.1367159256098504</v>
+        <v>0.03871859320679128</v>
       </c>
       <c r="B10">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -543,10 +543,10 @@
     </row>
     <row r="11">
       <c r="A11">
-        <v>0.1337776693127749</v>
+        <v>0.03606865756924983</v>
       </c>
       <c r="B11">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -561,10 +561,10 @@
     </row>
     <row r="12">
       <c r="A12">
-        <v>0.1176133185591873</v>
+        <v>0.0283186792374092</v>
       </c>
       <c r="B12">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -579,10 +579,10 @@
     </row>
     <row r="13">
       <c r="A13">
-        <v>0.09474360742810109</v>
+        <v>0.03204159002558448</v>
       </c>
       <c r="B13">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -597,10 +597,10 @@
     </row>
     <row r="14">
       <c r="A14">
-        <v>0.07069216672148865</v>
+        <v>0.02596447384893922</v>
       </c>
       <c r="B14">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -615,10 +615,10 @@
     </row>
     <row r="15">
       <c r="A15">
-        <v>0.049085736026836</v>
+        <v>0.02482569169579831</v>
       </c>
       <c r="B15">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -633,10 +633,10 @@
     </row>
     <row r="16">
       <c r="A16">
-        <v>0.03226170247274943</v>
+        <v>0.008245537161695831</v>
       </c>
       <c r="B16">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -651,10 +651,10 @@
     </row>
     <row r="17">
       <c r="A17">
-        <v>0.02039711328142171</v>
+        <v>0.003138673009819689</v>
       </c>
       <c r="B17">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -669,10 +669,10 @@
     </row>
     <row r="18">
       <c r="A18">
-        <v>0.0122587011585376</v>
+        <v>0.004087658137437123</v>
       </c>
       <c r="B18">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -687,10 +687,10 @@
     </row>
     <row r="19">
       <c r="A19">
-        <v>0.006953347753789159</v>
+        <v>0.0003049592799108877</v>
       </c>
       <c r="B19">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -705,10 +705,10 @@
     </row>
     <row r="20">
       <c r="A20">
-        <v>0.003888369301103059</v>
+        <v>3.611359893681565e-006</v>
       </c>
       <c r="B20">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -723,10 +723,10 @@
     </row>
     <row r="21">
       <c r="A21">
-        <v>0.002060296099352595</v>
+        <v>6.46032158758591e-005</v>
       </c>
       <c r="B21">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -741,14 +741,14 @@
     </row>
     <row r="22">
       <c r="A22">
-        <v>0.001103816671239376</v>
+        <v>0.006248807139752599</v>
       </c>
       <c r="B22">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>SO</t>
+          <t>NJ</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -759,14 +759,14 @@
     </row>
     <row r="23">
       <c r="A23">
-        <v>0.0005350827862503429</v>
+        <v>0.001433641088647649</v>
       </c>
       <c r="B23">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>SO</t>
+          <t>NJ</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -777,14 +777,14 @@
     </row>
     <row r="24">
       <c r="A24">
-        <v>0.0002883080621666154</v>
+        <v>0.02792318489381166</v>
       </c>
       <c r="B24">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>SO</t>
+          <t>NJ</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -795,14 +795,14 @@
     </row>
     <row r="25">
       <c r="A25">
-        <v>0.0001264189925588629</v>
+        <v>0.07346170951286946</v>
       </c>
       <c r="B25">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>SO</t>
+          <t>NJ</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -813,14 +813,14 @@
     </row>
     <row r="26">
       <c r="A26">
-        <v>6.245158865018167e-005</v>
+        <v>0.1557731010093097</v>
       </c>
       <c r="B26">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>SO</t>
+          <t>NJ</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -831,14 +831,14 @@
     </row>
     <row r="27">
       <c r="A27">
-        <v>3.061946822169101e-005</v>
+        <v>0.1669709540276506</v>
       </c>
       <c r="B27">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>SO</t>
+          <t>NJ</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -849,14 +849,14 @@
     </row>
     <row r="28">
       <c r="A28">
-        <v>1.394550037819591e-005</v>
+        <v>0.1230557561248669</v>
       </c>
       <c r="B28">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>SO</t>
+          <t>NJ</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -867,14 +867,14 @@
     </row>
     <row r="29">
       <c r="A29">
-        <v>6.972750189097953e-006</v>
+        <v>0.1121692976682281</v>
       </c>
       <c r="B29">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>SO</t>
+          <t>NJ</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -885,14 +885,14 @@
     </row>
     <row r="30">
       <c r="A30">
-        <v>2.728467465299199e-006</v>
+        <v>0.1035121862647952</v>
       </c>
       <c r="B30">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>SO</t>
+          <t>NJ</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -903,14 +903,14 @@
     </row>
     <row r="31">
       <c r="A31">
-        <v>9.09489155099733e-007</v>
+        <v>0.07377346469363562</v>
       </c>
       <c r="B31">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>SO</t>
+          <t>NJ</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -921,14 +921,14 @@
     </row>
     <row r="32">
       <c r="A32">
-        <v>6.063261033998221e-007</v>
+        <v>0.07330339774380486</v>
       </c>
       <c r="B32">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>SO</t>
+          <t>NJ</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -939,10 +939,10 @@
     </row>
     <row r="33">
       <c r="A33">
-        <v>8.953487705786961e-008</v>
+        <v>0.03382606819649087</v>
       </c>
       <c r="B33">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -957,10 +957,10 @@
     </row>
     <row r="34">
       <c r="A34">
-        <v>4.208139221719872e-006</v>
+        <v>0.02064670357662889</v>
       </c>
       <c r="B34">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -975,10 +975,10 @@
     </row>
     <row r="35">
       <c r="A35">
-        <v>9.633952771426771e-005</v>
+        <v>0.01203602187767675</v>
       </c>
       <c r="B35">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -993,10 +993,10 @@
     </row>
     <row r="36">
       <c r="A36">
-        <v>0.0008909615616028606</v>
+        <v>0.005441471210382728</v>
       </c>
       <c r="B36">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1011,10 +1011,10 @@
     </row>
     <row r="37">
       <c r="A37">
-        <v>0.004885739171293829</v>
+        <v>0.002759457077180684</v>
       </c>
       <c r="B37">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1029,10 +1029,10 @@
     </row>
     <row r="38">
       <c r="A38">
-        <v>0.01656780225541937</v>
+        <v>0.001004504402572765</v>
       </c>
       <c r="B38">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1047,10 +1047,10 @@
     </row>
     <row r="39">
       <c r="A39">
-        <v>0.04061257255906437</v>
+        <v>0.004915057531813137</v>
       </c>
       <c r="B39">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1065,10 +1065,10 @@
     </row>
     <row r="40">
       <c r="A40">
-        <v>0.07491687582013948</v>
+        <v>0.0004447334605897907</v>
       </c>
       <c r="B40">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1083,10 +1083,10 @@
     </row>
     <row r="41">
       <c r="A41">
-        <v>0.1114943800748368</v>
+        <v>0.0009518540192392074</v>
       </c>
       <c r="B41">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1101,10 +1101,10 @@
     </row>
     <row r="42">
       <c r="A42">
-        <v>0.1375617432512191</v>
+        <v>0.0003486284800528523</v>
       </c>
       <c r="B42">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1119,14 +1119,14 @@
     </row>
     <row r="43">
       <c r="A43">
-        <v>0.1458144414742741</v>
+        <v>0.002254149725674043</v>
       </c>
       <c r="B43">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>NJ</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1137,14 +1137,14 @@
     </row>
     <row r="44">
       <c r="A44">
-        <v>0.1348603864755061</v>
+        <v>0.01939381611391715</v>
       </c>
       <c r="B44">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>NJ</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1155,14 +1155,14 @@
     </row>
     <row r="45">
       <c r="A45">
-        <v>0.1114221254290511</v>
+        <v>0.03082453149162687</v>
       </c>
       <c r="B45">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>NJ</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -1173,14 +1173,14 @@
     </row>
     <row r="46">
       <c r="A46">
-        <v>0.08329966821955957</v>
+        <v>0.01205826954016867</v>
       </c>
       <c r="B46">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>NJ</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1191,14 +1191,14 @@
     </row>
     <row r="47">
       <c r="A47">
-        <v>0.05695098645946147</v>
+        <v>0.01358636242419098</v>
       </c>
       <c r="B47">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>NJ</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -1209,14 +1209,14 @@
     </row>
     <row r="48">
       <c r="A48">
-        <v>0.0358907717476635</v>
+        <v>0.07255743386906512</v>
       </c>
       <c r="B48">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>NJ</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -1227,14 +1227,14 @@
     </row>
     <row r="49">
       <c r="A49">
-        <v>0.02122173563001037</v>
+        <v>0.09554029119954641</v>
       </c>
       <c r="B49">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>NJ</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -1245,14 +1245,14 @@
     </row>
     <row r="50">
       <c r="A50">
-        <v>0.0117123258725711</v>
+        <v>0.139610630120838</v>
       </c>
       <c r="B50">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>NJ</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -1263,14 +1263,14 @@
     </row>
     <row r="51">
       <c r="A51">
-        <v>0.006141734426661624</v>
+        <v>0.1706877248844195</v>
       </c>
       <c r="B51">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>NJ</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -1281,14 +1281,14 @@
     </row>
     <row r="52">
       <c r="A52">
-        <v>0.003052602098411007</v>
+        <v>0.1480543318355053</v>
       </c>
       <c r="B52">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>NJ</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -1299,14 +1299,14 @@
     </row>
     <row r="53">
       <c r="A53">
-        <v>0.001457448728748002</v>
+        <v>0.1156416448505923</v>
       </c>
       <c r="B53">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>NJ</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -1317,14 +1317,14 @@
     </row>
     <row r="54">
       <c r="A54">
-        <v>0.0006530673932601009</v>
+        <v>0.07452578567899178</v>
       </c>
       <c r="B54">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>NJ</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -1335,14 +1335,14 @@
     </row>
     <row r="55">
       <c r="A55">
-        <v>0.0002867802112163564</v>
+        <v>0.02362953142355592</v>
       </c>
       <c r="B55">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>NJ</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -1353,14 +1353,14 @@
     </row>
     <row r="56">
       <c r="A56">
-        <v>0.0001258860371433647</v>
+        <v>0.01517321656094313</v>
       </c>
       <c r="B56">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>NJ</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -1371,14 +1371,14 @@
     </row>
     <row r="57">
       <c r="A57">
-        <v>5.094534504592781e-005</v>
+        <v>0.01881681464758865</v>
       </c>
       <c r="B57">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>NJ</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -1389,14 +1389,14 @@
     </row>
     <row r="58">
       <c r="A58">
-        <v>1.835464979686327e-005</v>
+        <v>0.01491044264541358</v>
       </c>
       <c r="B58">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>NJ</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -1407,14 +1407,14 @@
     </row>
     <row r="59">
       <c r="A59">
-        <v>6.356976271108742e-006</v>
+        <v>0.009156344573583504</v>
       </c>
       <c r="B59">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>NJ</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -1425,14 +1425,14 @@
     </row>
     <row r="60">
       <c r="A60">
-        <v>2.775581188793958e-006</v>
+        <v>0.007934270683760751</v>
       </c>
       <c r="B60">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>NJ</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -1443,14 +1443,14 @@
     </row>
     <row r="61">
       <c r="A61">
-        <v>6.267441394050873e-007</v>
+        <v>0.00592587713432482</v>
       </c>
       <c r="B61">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>NJ</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -1461,14 +1461,14 @@
     </row>
     <row r="62">
       <c r="A62">
-        <v>1.790697541157392e-007</v>
+        <v>0.004986297716739929</v>
       </c>
       <c r="B62">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>NJ</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -1479,14 +1479,14 @@
     </row>
     <row r="63">
       <c r="A63">
-        <v>8.953487705786961e-008</v>
+        <v>0.002011096366852807</v>
       </c>
       <c r="B63">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>NJ</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -1497,10 +1497,10 @@
     </row>
     <row r="64">
       <c r="A64">
-        <v>2.965874939533225e-007</v>
+        <v>0.002519326145574147</v>
       </c>
       <c r="B64">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
@@ -1515,10 +1515,10 @@
     </row>
     <row r="65">
       <c r="A65">
-        <v>1.028169979038185e-005</v>
+        <v>0.0001991075497098175</v>
       </c>
       <c r="B65">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
@@ -1533,10 +1533,10 @@
     </row>
     <row r="66">
       <c r="A66">
-        <v>0.0001474039844948013</v>
+        <v>2.702817416875351e-006</v>
       </c>
       <c r="B66">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
@@ -1544,636 +1544,6 @@
         </is>
       </c>
       <c r="D66" t="inlineStr">
-        <is>
-          <t>y2</t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67">
-        <v>0.001041318691270115</v>
-      </c>
-      <c r="B67">
-        <v>6</v>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="D67" t="inlineStr">
-        <is>
-          <t>y2</t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68">
-        <v>0.004535020507542269</v>
-      </c>
-      <c r="B68">
-        <v>7</v>
-      </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="D68" t="inlineStr">
-        <is>
-          <t>y2</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69">
-        <v>0.01364302472185283</v>
-      </c>
-      <c r="B69">
-        <v>8</v>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="D69" t="inlineStr">
-        <is>
-          <t>y2</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70">
-        <v>0.03098756023074112</v>
-      </c>
-      <c r="B70">
-        <v>9</v>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="D70" t="inlineStr">
-        <is>
-          <t>y2</t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71">
-        <v>0.05605711246963562</v>
-      </c>
-      <c r="B71">
-        <v>10</v>
-      </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="D71" t="inlineStr">
-        <is>
-          <t>y2</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72">
-        <v>0.08436006156760925</v>
-      </c>
-      <c r="B72">
-        <v>11</v>
-      </c>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="D72" t="inlineStr">
-        <is>
-          <t>y2</t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73">
-        <v>0.1088147879315385</v>
-      </c>
-      <c r="B73">
-        <v>12</v>
-      </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="D73" t="inlineStr">
-        <is>
-          <t>y2</t>
-        </is>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74">
-        <v>0.1233106994235031</v>
-      </c>
-      <c r="B74">
-        <v>13</v>
-      </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="D74" t="inlineStr">
-        <is>
-          <t>y2</t>
-        </is>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75">
-        <v>0.1251313511863846</v>
-      </c>
-      <c r="B75">
-        <v>14</v>
-      </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="D75" t="inlineStr">
-        <is>
-          <t>y2</t>
-        </is>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76">
-        <v>0.1151857838891498</v>
-      </c>
-      <c r="B76">
-        <v>15</v>
-      </c>
-      <c r="C76" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="D76" t="inlineStr">
-        <is>
-          <t>y2</t>
-        </is>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77">
-        <v>0.09758984104788712</v>
-      </c>
-      <c r="B77">
-        <v>16</v>
-      </c>
-      <c r="C77" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="D77" t="inlineStr">
-        <is>
-          <t>y2</t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78">
-        <v>0.07706084561642201</v>
-      </c>
-      <c r="B78">
-        <v>17</v>
-      </c>
-      <c r="C78" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="D78" t="inlineStr">
-        <is>
-          <t>y2</t>
-        </is>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79">
-        <v>0.05701469462511291</v>
-      </c>
-      <c r="B79">
-        <v>18</v>
-      </c>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="D79" t="inlineStr">
-        <is>
-          <t>y2</t>
-        </is>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80">
-        <v>0.0396748056536299</v>
-      </c>
-      <c r="B80">
-        <v>19</v>
-      </c>
-      <c r="C80" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="D80" t="inlineStr">
-        <is>
-          <t>y2</t>
-        </is>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81">
-        <v>0.02619332225348364</v>
-      </c>
-      <c r="B81">
-        <v>20</v>
-      </c>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="D81" t="inlineStr">
-        <is>
-          <t>y2</t>
-        </is>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82">
-        <v>0.0164980748011455</v>
-      </c>
-      <c r="B82">
-        <v>21</v>
-      </c>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="D82" t="inlineStr">
-        <is>
-          <t>y2</t>
-        </is>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83">
-        <v>0.009992724708773325</v>
-      </c>
-      <c r="B83">
-        <v>22</v>
-      </c>
-      <c r="C83" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="D83" t="inlineStr">
-        <is>
-          <t>y2</t>
-        </is>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84">
-        <v>0.005828636293668678</v>
-      </c>
-      <c r="B84">
-        <v>23</v>
-      </c>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="D84" t="inlineStr">
-        <is>
-          <t>y2</t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85">
-        <v>0.003260485183526858</v>
-      </c>
-      <c r="B85">
-        <v>24</v>
-      </c>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="D85" t="inlineStr">
-        <is>
-          <t>y2</t>
-        </is>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86">
-        <v>0.001792673675951866</v>
-      </c>
-      <c r="B86">
-        <v>25</v>
-      </c>
-      <c r="C86" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="D86" t="inlineStr">
-        <is>
-          <t>y2</t>
-        </is>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87">
-        <v>0.0009433459557675343</v>
-      </c>
-      <c r="B87">
-        <v>26</v>
-      </c>
-      <c r="C87" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="D87" t="inlineStr">
-        <is>
-          <t>y2</t>
-        </is>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88">
-        <v>0.000476121790293067</v>
-      </c>
-      <c r="B88">
-        <v>27</v>
-      </c>
-      <c r="C88" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="D88" t="inlineStr">
-        <is>
-          <t>y2</t>
-        </is>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89">
-        <v>0.0002325245952594048</v>
-      </c>
-      <c r="B89">
-        <v>28</v>
-      </c>
-      <c r="C89" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="D89" t="inlineStr">
-        <is>
-          <t>y2</t>
-        </is>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90">
-        <v>0.0001138895976780758</v>
-      </c>
-      <c r="B90">
-        <v>29</v>
-      </c>
-      <c r="C90" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="D90" t="inlineStr">
-        <is>
-          <t>y2</t>
-        </is>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91">
-        <v>5.743911132896012e-005</v>
-      </c>
-      <c r="B91">
-        <v>30</v>
-      </c>
-      <c r="C91" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="D91" t="inlineStr">
-        <is>
-          <t>y2</t>
-        </is>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92">
-        <v>2.392472451223468e-005</v>
-      </c>
-      <c r="B92">
-        <v>31</v>
-      </c>
-      <c r="C92" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="D92" t="inlineStr">
-        <is>
-          <t>y2</t>
-        </is>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93">
-        <v>1.057828728433517e-005</v>
-      </c>
-      <c r="B93">
-        <v>32</v>
-      </c>
-      <c r="C93" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="D93" t="inlineStr">
-        <is>
-          <t>y2</t>
-        </is>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94">
-        <v>5.338574891159804e-006</v>
-      </c>
-      <c r="B94">
-        <v>33</v>
-      </c>
-      <c r="C94" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="D94" t="inlineStr">
-        <is>
-          <t>y2</t>
-        </is>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95">
-        <v>3.262462433486547e-006</v>
-      </c>
-      <c r="B95">
-        <v>34</v>
-      </c>
-      <c r="C95" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="D95" t="inlineStr">
-        <is>
-          <t>y2</t>
-        </is>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96">
-        <v>1.680662465735494e-006</v>
-      </c>
-      <c r="B96">
-        <v>35</v>
-      </c>
-      <c r="C96" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="D96" t="inlineStr">
-        <is>
-          <t>y2</t>
-        </is>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97">
-        <v>4.943124899222041e-007</v>
-      </c>
-      <c r="B97">
-        <v>36</v>
-      </c>
-      <c r="C97" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="D97" t="inlineStr">
-        <is>
-          <t>y2</t>
-        </is>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98">
-        <v>1.977249959688816e-007</v>
-      </c>
-      <c r="B98">
-        <v>37</v>
-      </c>
-      <c r="C98" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="D98" t="inlineStr">
-        <is>
-          <t>y2</t>
-        </is>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99">
-        <v>1.977249959688816e-007</v>
-      </c>
-      <c r="B99">
-        <v>38</v>
-      </c>
-      <c r="C99" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="D99" t="inlineStr">
-        <is>
-          <t>y2</t>
-        </is>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100">
-        <v>9.886249798444082e-008</v>
-      </c>
-      <c r="B100">
-        <v>39</v>
-      </c>
-      <c r="C100" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="D100" t="inlineStr">
-        <is>
-          <t>y2</t>
-        </is>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101">
-        <v>9.886249798444082e-008</v>
-      </c>
-      <c r="B101">
-        <v>40</v>
-      </c>
-      <c r="C101" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="D101" t="inlineStr">
         <is>
           <t>y2</t>
         </is>

</xml_diff>